<commit_message>
Example for sample file
</commit_message>
<xml_diff>
--- a/wingdiscs.xlsx
+++ b/wingdiscs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheti00/PycharmProjects/Shinya/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheti00/PycharmProjects/Wingdisc-alignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF089490-EEEE-CB42-B32D-7DD22634E9CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E439108D-0386-6D4C-AD47-2F888FC5FE86}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="2860" windowWidth="28800" windowHeight="27240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="2860" windowWidth="28800" windowHeight="27240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample1" sheetId="4" r:id="rId1"/>
@@ -19325,7 +19325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C581783-EC93-4A4E-91BE-1AD412BF6088}">
   <dimension ref="A1:E419"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -22518,7 +22518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6969CE1-4A8D-8D49-8C0B-9FE6CA8A35F3}">
   <dimension ref="A1:E540"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improving the user interface and compatibility with jupyter notebook, additionally rewriting the script to be more modular/ definition of functions
</commit_message>
<xml_diff>
--- a/wingdiscs.xlsx
+++ b/wingdiscs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheti00/PycharmProjects/Wingdisc-alignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E439108D-0386-6D4C-AD47-2F888FC5FE86}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA03EE8F-065E-274B-A19E-F5D3C459D7A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="2860" windowWidth="28800" windowHeight="27240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample1" sheetId="4" r:id="rId1"/>
     <sheet name="sheet" sheetId="5" r:id="rId2"/>
-    <sheet name="sample3" sheetId="6" r:id="rId3"/>
+    <sheet name="any name you want" sheetId="6" r:id="rId3"/>
     <sheet name="sample4" sheetId="7" r:id="rId4"/>
     <sheet name="sample5" sheetId="8" r:id="rId5"/>
   </sheets>
@@ -15424,7 +15424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC588FD8-2500-3042-9547-4AACA23B47CE}">
   <dimension ref="A1:E538"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -22518,7 +22518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6969CE1-4A8D-8D49-8C0B-9FE6CA8A35F3}">
   <dimension ref="A1:E540"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>